<commit_message>
fourth commit Write Operation
</commit_message>
<xml_diff>
--- a/ReadFromExcel/input.xlsx
+++ b/ReadFromExcel/input.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tenant\eclipse-workspace\ReadFromExcel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tenant\git\Test-project\ReadFromExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7D4512C-03D3-415C-8A79-DBBCC359B84C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58D13E1E-BB01-4C77-9C53-719EDB229935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4AAA39C0-054C-40F0-ACAE-6FE699F76C81}"/>
+    <workbookView xWindow="3045" yWindow="1980" windowWidth="15375" windowHeight="7875" xr2:uid="{4AAA39C0-054C-40F0-ACAE-6FE699F76C81}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,12 +34,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>swapnil</t>
-  </si>
-  <si>
-    <t>kumar</t>
+    <t>Swapnil</t>
   </si>
 </sst>
 </file>
@@ -391,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0935E6B1-F4B1-4676-9980-80C8D05C9A3E}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -403,15 +400,12 @@
     <col min="2" max="2" width="6.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>123</v>
       </c>

</xml_diff>